<commit_message>
add attempt for production equilibrium
</commit_message>
<xml_diff>
--- a/Data/output/temp.xlsx
+++ b/Data/output/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Tobin\sam\Optimal-Unilateral-Carbon-Policy\Data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35549FFB-1BCF-4298-84A3-D47D0343D974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3986DBD3-7E6D-477D-B476-91ED94B0E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15732" yWindow="2496" windowWidth="15384" windowHeight="11088" xr2:uid="{36D558F1-4F96-478A-B61D-823EAD2C98E9}"/>
+    <workbookView xWindow="14424" yWindow="2760" windowWidth="15384" windowHeight="11088" xr2:uid="{36D558F1-4F96-478A-B61D-823EAD2C98E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>PC_hybrid</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t>EPC_hybrid</t>
+  </si>
+  <si>
+    <t>puretc</t>
+  </si>
+  <si>
+    <t>purete</t>
+  </si>
+  <si>
+    <t>EC_hybrid</t>
   </si>
 </sst>
 </file>
@@ -545,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3496870A-4D61-430B-B032-0A96A329A70C}">
   <dimension ref="A1:AV18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,9 +703,301 @@
         <v>48</v>
       </c>
     </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1.00000021739919</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="J2">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K2">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="L2">
+        <v>4.4800452869790401</v>
+      </c>
+      <c r="M2">
+        <v>27.795949021407999</v>
+      </c>
+      <c r="N2">
+        <v>32.275994308386998</v>
+      </c>
+      <c r="O2">
+        <v>4.5984020003110899</v>
+      </c>
+      <c r="P2">
+        <v>0.42160093834429402</v>
+      </c>
+      <c r="Q2">
+        <v>1.1961107399664801</v>
+      </c>
+      <c r="R2">
+        <v>26.0598683346055</v>
+      </c>
+      <c r="S2">
+        <v>5.0200029386553799</v>
+      </c>
+      <c r="T2">
+        <v>5.79451274027757</v>
+      </c>
+      <c r="U2">
+        <v>27.255979074572</v>
+      </c>
+      <c r="V2">
+        <v>26.481469272949798</v>
+      </c>
+      <c r="W2">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="X2">
+        <v>7.9740733333333296</v>
+      </c>
+      <c r="Y2">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0.42160093834429402</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD2">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE2">
+        <v>28.4466895033333</v>
+      </c>
+      <c r="AF2">
+        <v>154.45058166666601</v>
+      </c>
+      <c r="AG2">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH2">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>4.8697910023516202E-7</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>3.0214083513774501E-6</v>
+      </c>
+      <c r="AK2">
+        <v>-0.70128518425964304</v>
+      </c>
+      <c r="AL2">
+        <v>1.3753239661330099</v>
+      </c>
+      <c r="AM2">
+        <v>1.09717397864432</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>3.0214080197765699E-6</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>-5.9254279918263802E-6</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>-4.7270501823959404E-6</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>4.3083870693294498E-6</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>-6.1103817250440699E-7</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>-3.0619896362334298E-5</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>-3.0619896362334298E-5</v>
+      </c>
+      <c r="AV2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.99999966741491597</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.77078593725241795</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="J3">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K3">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="L3">
+        <v>4.4800440550019003</v>
+      </c>
+      <c r="M3">
+        <v>27.795941377740998</v>
+      </c>
+      <c r="N3">
+        <v>32.275985432742999</v>
+      </c>
+      <c r="O3">
+        <v>4.5984045293607503</v>
+      </c>
+      <c r="P3">
+        <v>0.42160117021825999</v>
+      </c>
+      <c r="Q3">
+        <v>1.1961113978088</v>
+      </c>
+      <c r="R3">
+        <v>26.0598826671282</v>
+      </c>
+      <c r="S3">
+        <v>5.0200056995790101</v>
+      </c>
+      <c r="T3">
+        <v>5.7945159271695603</v>
+      </c>
+      <c r="U3">
+        <v>27.255994064936999</v>
+      </c>
+      <c r="V3">
+        <v>26.481483837346499</v>
+      </c>
+      <c r="W3">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="X3">
+        <v>7.9740733333333296</v>
+      </c>
+      <c r="Y3">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0.42160117021825999</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD3">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE3">
+        <v>28.4466895033333</v>
+      </c>
+      <c r="AF3">
+        <v>154.45058166666601</v>
+      </c>
+      <c r="AG3">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH3">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>-7.44997975873844E-7</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>-4.6222581317710596E-6</v>
+      </c>
+      <c r="AK3">
+        <v>-1.0120426552933699</v>
+      </c>
+      <c r="AL3">
+        <v>1.98476614578185</v>
+      </c>
+      <c r="AM3">
+        <v>2.15388503924502</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>-4.62225890274226E-6</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>9.0649370747541895E-6</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>9.8373465249323999E-6</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>-4.5672570010424301E-6</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>9.3478809315428095E-7</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>3.8308054920663503E-5</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>3.8308054920663503E-5</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -705,79 +1006,79 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E4">
-        <v>0.99999966741491597</v>
+        <v>0.96283308853786498</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.40419181689424899</v>
       </c>
       <c r="G4">
-        <v>0.77078593725241795</v>
+        <v>0.45647989020118301</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.40419181689424899</v>
       </c>
       <c r="I4">
-        <v>1.5920602214279201E-2</v>
+        <v>1.4099641462562301E-2</v>
       </c>
       <c r="J4">
         <v>0.79357871945774905</v>
       </c>
       <c r="K4">
-        <v>1.5920602214279201E-2</v>
+        <v>1.2940097471930499E-2</v>
       </c>
       <c r="L4">
-        <v>4.4800440550019003</v>
+        <v>4.3960017869681502</v>
       </c>
       <c r="M4">
-        <v>27.795941377740998</v>
+        <v>27.274510354555002</v>
       </c>
       <c r="N4">
-        <v>32.275985432742999</v>
+        <v>31.670512141523101</v>
       </c>
       <c r="O4">
-        <v>4.5984045293607503</v>
+        <v>3.3638025851585298</v>
       </c>
       <c r="P4">
-        <v>0.42160117021825999</v>
+        <v>0.31574905245203699</v>
       </c>
       <c r="Q4">
-        <v>1.1961113978088</v>
+        <v>0.87497361017217501</v>
       </c>
       <c r="R4">
-        <v>26.0598826671282</v>
+        <v>27.115910366483401</v>
       </c>
       <c r="S4">
-        <v>5.0200056995790101</v>
+        <v>3.6795516376105701</v>
       </c>
       <c r="T4">
-        <v>5.7945159271695603</v>
+        <v>4.2387761953307104</v>
       </c>
       <c r="U4">
-        <v>27.255994064936999</v>
+        <v>27.990883976655599</v>
       </c>
       <c r="V4">
-        <v>26.481483837346499</v>
+        <v>27.4316594189354</v>
       </c>
       <c r="W4">
-        <v>2.8106735333333299</v>
+        <v>2.4891953554853199</v>
       </c>
       <c r="X4">
-        <v>7.9740733333333296</v>
+        <v>7.6204158768045298</v>
       </c>
       <c r="Y4">
-        <v>2.8106735333333299</v>
+        <v>2.28448578725797</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>0.20470956822734701</v>
       </c>
       <c r="AA4">
-        <v>0.42160117021825999</v>
+        <v>0.25067047832485401</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>2.27117535886792E-2</v>
       </c>
       <c r="AC4">
         <v>38.630093333333299</v>
@@ -786,10 +1087,10 @@
         <v>176.54316686666601</v>
       </c>
       <c r="AE4">
-        <v>28.4466895033333</v>
+        <v>28.173433052162501</v>
       </c>
       <c r="AF4">
-        <v>154.45058166666601</v>
+        <v>154.723838117837</v>
       </c>
       <c r="AG4">
         <v>5.7945140000000004</v>
@@ -797,365 +1098,365 @@
       <c r="AH4">
         <v>26.481475029999999</v>
       </c>
-      <c r="AI4" s="1">
-        <v>-7.44997975873844E-7</v>
-      </c>
-      <c r="AJ4" s="1">
-        <v>-4.6222581317710596E-6</v>
+      <c r="AI4">
+        <v>-8.2476274078490702E-2</v>
+      </c>
+      <c r="AJ4">
+        <v>-0.51171498565526097</v>
       </c>
       <c r="AK4">
-        <v>-1.0120426552933699</v>
+        <v>-0.86119688465030597</v>
       </c>
       <c r="AL4">
-        <v>1.98476614578185</v>
+        <v>1.2137503731422901</v>
       </c>
       <c r="AM4">
-        <v>2.15388503924502</v>
-      </c>
-      <c r="AN4" s="1">
-        <v>-4.62225890274226E-6</v>
-      </c>
-      <c r="AO4" s="1">
-        <v>9.0649370747541895E-6</v>
-      </c>
-      <c r="AP4" s="1">
-        <v>9.8373465249323999E-6</v>
-      </c>
-      <c r="AQ4" s="1">
-        <v>-4.5672570010424301E-6</v>
-      </c>
-      <c r="AR4" s="1">
-        <v>9.3478809315428095E-7</v>
+        <v>1.5693148901032401</v>
+      </c>
+      <c r="AN4">
+        <v>-0.52143564544497401</v>
+      </c>
+      <c r="AO4">
+        <v>0.73489897665563497</v>
+      </c>
+      <c r="AP4">
+        <v>0.95018541893549702</v>
+      </c>
+      <c r="AQ4">
+        <v>-0.60547785847681701</v>
+      </c>
+      <c r="AR4">
+        <v>-1.0315880978115399</v>
       </c>
       <c r="AS4">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="1">
-        <v>3.8308054920663503E-5</v>
-      </c>
-      <c r="AU4" s="1">
-        <v>3.8308054920663503E-5</v>
+        <v>5.9238961929218299E-2</v>
+      </c>
+      <c r="AT4">
+        <v>0.95788833621003999</v>
+      </c>
+      <c r="AU4">
+        <v>-0.76622263877436303</v>
       </c>
       <c r="AV4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>66</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E6">
-        <v>0.96283308853786498</v>
-      </c>
-      <c r="F6">
-        <v>0.40419181689424899</v>
-      </c>
-      <c r="G6">
-        <v>0.45647989020118301</v>
-      </c>
-      <c r="H6">
-        <v>0.40419181689424899</v>
-      </c>
-      <c r="I6">
-        <v>1.4099641462562301E-2</v>
-      </c>
-      <c r="J6">
+      <c r="E5">
+        <v>0.97576131052849402</v>
+      </c>
+      <c r="F5">
+        <v>0.31414642065147902</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.5296800941034702E-8</v>
+      </c>
+      <c r="H5">
+        <v>0.31414642065147902</v>
+      </c>
+      <c r="I5">
+        <v>1.34988851109269E-2</v>
+      </c>
+      <c r="J5">
+        <v>0.76479832358213595</v>
+      </c>
+      <c r="K5">
+        <v>1.34988851109269E-2</v>
+      </c>
+      <c r="L5">
+        <v>4.4254165326199004</v>
+      </c>
+      <c r="M5">
+        <v>27.457010913866299</v>
+      </c>
+      <c r="N5">
+        <v>31.882427446486201</v>
+      </c>
+      <c r="O5">
+        <v>3.4356213906240201</v>
+      </c>
+      <c r="P5">
+        <v>0.27712865064452702</v>
+      </c>
+      <c r="Q5">
+        <v>1.39673441867521</v>
+      </c>
+      <c r="R5">
+        <v>26.7729457595042</v>
+      </c>
+      <c r="S5">
+        <v>3.7127500412685501</v>
+      </c>
+      <c r="T5">
+        <v>4.83235580929923</v>
+      </c>
+      <c r="U5">
+        <v>28.169680178179402</v>
+      </c>
+      <c r="V5">
+        <v>27.050074410148699</v>
+      </c>
+      <c r="W5">
+        <v>2.3831359266523302</v>
+      </c>
+      <c r="X5">
+        <v>9.08586271217853</v>
+      </c>
+      <c r="Y5">
+        <v>2.3831359266523302</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0.27712865064452702</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>-5.2063541433542898E-17</v>
+      </c>
+      <c r="AC5">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD5">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE5">
+        <v>27.138261565636</v>
+      </c>
+      <c r="AF5">
+        <v>155.759009604363</v>
+      </c>
+      <c r="AG5">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH5">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI5">
+        <v>-5.3964854832110998E-2</v>
+      </c>
+      <c r="AJ5">
+        <v>-0.33481901583019702</v>
+      </c>
+      <c r="AK5">
+        <v>-0.86119749734222495</v>
+      </c>
+      <c r="AL5">
+        <v>2.3216008993283799</v>
+      </c>
+      <c r="AM5">
+        <v>1.44475231465061</v>
+      </c>
+      <c r="AN5">
+        <v>-0.33893508613364098</v>
+      </c>
+      <c r="AO5">
+        <v>0.913695178179455</v>
+      </c>
+      <c r="AP5">
+        <v>0.56860041014877105</v>
+      </c>
+      <c r="AQ5">
+        <v>-0.39356255351373098</v>
+      </c>
+      <c r="AR5">
+        <v>-0.81483598713626604</v>
+      </c>
+      <c r="AS5">
+        <v>4.60677814494612E-2</v>
+      </c>
+      <c r="AT5">
+        <v>0.63330330171501703</v>
+      </c>
+      <c r="AU5">
+        <v>-0.48737437188795901</v>
+      </c>
+      <c r="AV5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1.0405061959524999</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.68633053944338496</v>
+      </c>
+      <c r="I9">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="J9">
         <v>0.79357871945774905</v>
       </c>
-      <c r="K6">
-        <v>1.2940097471930499E-2</v>
-      </c>
-      <c r="L6">
-        <v>4.3960017869681502</v>
-      </c>
-      <c r="M6">
-        <v>27.274510354555002</v>
-      </c>
-      <c r="N6">
-        <v>31.670512141523101</v>
-      </c>
-      <c r="O6">
-        <v>3.3638025851585298</v>
-      </c>
-      <c r="P6">
-        <v>0.31574905245203699</v>
-      </c>
-      <c r="Q6">
-        <v>0.87497361017217501</v>
-      </c>
-      <c r="R6">
-        <v>27.115910366483401</v>
-      </c>
-      <c r="S6">
-        <v>3.6795516376105701</v>
-      </c>
-      <c r="T6">
-        <v>4.2387761953307104</v>
-      </c>
-      <c r="U6">
-        <v>27.990883976655599</v>
-      </c>
-      <c r="V6">
-        <v>27.4316594189354</v>
-      </c>
-      <c r="W6">
-        <v>2.4891953554853199</v>
-      </c>
-      <c r="X6">
-        <v>7.6204158768045298</v>
-      </c>
-      <c r="Y6">
-        <v>2.28448578725797</v>
-      </c>
-      <c r="Z6">
-        <v>0.20470956822734701</v>
-      </c>
-      <c r="AA6">
-        <v>0.25067047832485401</v>
-      </c>
-      <c r="AB6">
-        <v>2.27117535886792E-2</v>
-      </c>
-      <c r="AC6">
+      <c r="K9">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="L9">
+        <v>2.6661937787890402</v>
+      </c>
+      <c r="M9">
+        <v>28.353311852176699</v>
+      </c>
+      <c r="N9">
+        <v>31.0195056309657</v>
+      </c>
+      <c r="O9">
+        <v>4.4193903101081498</v>
+      </c>
+      <c r="P9">
+        <v>0.40518838968955401</v>
+      </c>
+      <c r="Q9">
+        <v>1.14954721524272</v>
+      </c>
+      <c r="R9">
+        <v>25.045380893810101</v>
+      </c>
+      <c r="S9">
+        <v>4.8245786997977103</v>
+      </c>
+      <c r="T9">
+        <v>5.5689375253508704</v>
+      </c>
+      <c r="U9">
+        <v>26.194928109052899</v>
+      </c>
+      <c r="V9">
+        <v>25.4505692834997</v>
+      </c>
+      <c r="W9">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="X9">
+        <v>7.9740733333333296</v>
+      </c>
+      <c r="Y9">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0.40518838968955401</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
         <v>38.630093333333299</v>
       </c>
-      <c r="AD6">
+      <c r="AD9">
         <v>176.54316686666601</v>
       </c>
-      <c r="AE6">
-        <v>28.173433052162501</v>
-      </c>
-      <c r="AF6">
-        <v>154.723838117837</v>
-      </c>
-      <c r="AG6">
+      <c r="AE9">
+        <v>28.4466895033333</v>
+      </c>
+      <c r="AF9">
+        <v>154.45058166666601</v>
+      </c>
+      <c r="AG9">
         <v>5.7945140000000004</v>
       </c>
-      <c r="AH6">
+      <c r="AH9">
         <v>26.481475029999999</v>
       </c>
-      <c r="AI6">
-        <v>-8.2476274078490702E-2</v>
-      </c>
-      <c r="AJ6">
-        <v>-0.51171498565526097</v>
-      </c>
-      <c r="AK6">
-        <v>-0.86119688465030597</v>
-      </c>
-      <c r="AL6">
-        <v>1.2137503731422901</v>
-      </c>
-      <c r="AM6">
-        <v>1.5693148901032401</v>
-      </c>
-      <c r="AN6">
-        <v>-0.52143564544497401</v>
-      </c>
-      <c r="AO6">
-        <v>0.73489897665563497</v>
-      </c>
-      <c r="AP6">
-        <v>0.95018541893549702</v>
-      </c>
-      <c r="AQ6">
-        <v>-0.60547785847681701</v>
-      </c>
-      <c r="AR6">
-        <v>-1.0315880978115399</v>
-      </c>
-      <c r="AS6">
-        <v>5.9238961929218299E-2</v>
-      </c>
-      <c r="AT6">
-        <v>0.95788833621003999</v>
-      </c>
-      <c r="AU6">
-        <v>-0.76622263877436303</v>
-      </c>
-      <c r="AV6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.97576131052849402</v>
-      </c>
-      <c r="F7">
-        <v>0.31414642065147902</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3.5296800941034702E-8</v>
-      </c>
-      <c r="H7">
-        <v>0.31414642065147902</v>
-      </c>
-      <c r="I7">
-        <v>1.34988851109269E-2</v>
-      </c>
-      <c r="J7">
-        <v>0.76479832358213595</v>
-      </c>
-      <c r="K7">
-        <v>1.34988851109269E-2</v>
-      </c>
-      <c r="L7">
-        <v>4.4254165326199004</v>
-      </c>
-      <c r="M7">
-        <v>27.457010913866299</v>
-      </c>
-      <c r="N7">
-        <v>31.882427446486201</v>
-      </c>
-      <c r="O7">
-        <v>3.4356213906240201</v>
-      </c>
-      <c r="P7">
-        <v>0.27712865064452702</v>
-      </c>
-      <c r="Q7">
-        <v>1.39673441867521</v>
-      </c>
-      <c r="R7">
-        <v>26.7729457595042</v>
-      </c>
-      <c r="S7">
-        <v>3.7127500412685501</v>
-      </c>
-      <c r="T7">
-        <v>4.83235580929923</v>
-      </c>
-      <c r="U7">
-        <v>28.169680178179402</v>
-      </c>
-      <c r="V7">
-        <v>27.050074410148699</v>
-      </c>
-      <c r="W7">
-        <v>2.3831359266523302</v>
-      </c>
-      <c r="X7">
-        <v>9.08586271217853</v>
-      </c>
-      <c r="Y7">
-        <v>2.3831359266523302</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0.27712865064452702</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>-5.2063541433542898E-17</v>
-      </c>
-      <c r="AC7">
-        <v>38.630093333333299</v>
-      </c>
-      <c r="AD7">
-        <v>176.54316686666601</v>
-      </c>
-      <c r="AE7">
-        <v>27.138261565636</v>
-      </c>
-      <c r="AF7">
-        <v>155.759009604363</v>
-      </c>
-      <c r="AG7">
-        <v>5.7945140000000004</v>
-      </c>
-      <c r="AH7">
-        <v>26.481475029999999</v>
-      </c>
-      <c r="AI7">
-        <v>-5.3964854832110998E-2</v>
-      </c>
-      <c r="AJ7">
-        <v>-0.33481901583019702</v>
-      </c>
-      <c r="AK7">
-        <v>-0.86119749734222495</v>
-      </c>
-      <c r="AL7">
-        <v>2.3216008993283799</v>
-      </c>
-      <c r="AM7">
-        <v>1.44475231465061</v>
-      </c>
-      <c r="AN7">
-        <v>-0.33893508613364098</v>
-      </c>
-      <c r="AO7">
-        <v>0.913695178179455</v>
-      </c>
-      <c r="AP7">
-        <v>0.56860041014877105</v>
-      </c>
-      <c r="AQ7">
-        <v>-0.39356255351373098</v>
-      </c>
-      <c r="AR7">
-        <v>-0.81483598713626604</v>
-      </c>
-      <c r="AS7">
-        <v>4.60677814494612E-2</v>
-      </c>
-      <c r="AT7">
-        <v>0.63330330171501703</v>
-      </c>
-      <c r="AU7">
-        <v>-0.48737437188795901</v>
-      </c>
-      <c r="AV7">
+      <c r="AI9">
+        <v>-1.17858128933895</v>
+      </c>
+      <c r="AJ9">
+        <v>0.56861688598782201</v>
+      </c>
+      <c r="AK9">
+        <v>0.44359155267892397</v>
+      </c>
+      <c r="AL9">
+        <v>-0.84446485535083404</v>
+      </c>
+      <c r="AM9">
+        <v>-0.82046760143353104</v>
+      </c>
+      <c r="AN9">
+        <v>0.55736585217670098</v>
+      </c>
+      <c r="AO9">
+        <v>-1.0610568909470901</v>
+      </c>
+      <c r="AP9">
+        <v>-1.0309047165002501</v>
+      </c>
+      <c r="AQ9">
+        <v>-1.25648436903425</v>
+      </c>
+      <c r="AR9">
+        <v>-0.11384969289972</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>1.5139866998404301</v>
+      </c>
+      <c r="AU9">
+        <v>-1.738618524911</v>
+      </c>
+      <c r="AV9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>1.00000021739919</v>
+        <v>0.96680290503244404</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.36681367950521898</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.36681367950521898</v>
       </c>
       <c r="I10">
         <v>1.5920602214279201E-2</v>
@@ -1164,58 +1465,58 @@
         <v>0.79357871945774905</v>
       </c>
       <c r="K10">
-        <v>1.5920602214279201E-2</v>
+        <v>1.31631220587518E-2</v>
       </c>
       <c r="L10">
-        <v>4.4800452869790401</v>
+        <v>4.4050549496600002</v>
       </c>
       <c r="M10">
-        <v>27.795949021407999</v>
+        <v>27.330679708332799</v>
       </c>
       <c r="N10">
-        <v>32.275994308386998</v>
+        <v>31.735734657992801</v>
       </c>
       <c r="O10">
-        <v>4.5984020003110899</v>
+        <v>3.4480698891531798</v>
       </c>
       <c r="P10">
-        <v>0.42160093834429402</v>
+        <v>0.43607753742305</v>
       </c>
       <c r="Q10">
-        <v>1.1961107399664801</v>
+        <v>0.89689275237183497</v>
       </c>
       <c r="R10">
-        <v>26.0598683346055</v>
+        <v>26.954691451951501</v>
       </c>
       <c r="S10">
-        <v>5.0200029386553799</v>
+        <v>3.8841474265762299</v>
       </c>
       <c r="T10">
-        <v>5.79451274027757</v>
+        <v>4.3449626415250204</v>
       </c>
       <c r="U10">
-        <v>27.255979074572</v>
+        <v>27.851584204323402</v>
       </c>
       <c r="V10">
-        <v>26.481469272949798</v>
+        <v>27.3907689893746</v>
       </c>
       <c r="W10">
         <v>2.8106735333333299</v>
       </c>
       <c r="X10">
-        <v>7.9740733333333296</v>
+        <v>7.6450808518289604</v>
       </c>
       <c r="Y10">
-        <v>2.8106735333333299</v>
+        <v>2.32385925410453</v>
       </c>
       <c r="Z10">
-        <v>0</v>
+        <v>0.48681427922878601</v>
       </c>
       <c r="AA10">
-        <v>0.42160093834429402</v>
+        <v>0.261378649958729</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>5.6139641927635597E-2</v>
       </c>
       <c r="AC10">
         <v>38.630093333333299</v>
@@ -1235,44 +1536,44 @@
       <c r="AH10">
         <v>26.481475029999999</v>
       </c>
-      <c r="AI10" s="1">
-        <v>4.8697910023516202E-7</v>
-      </c>
-      <c r="AJ10" s="1">
-        <v>3.0214083513774501E-6</v>
+      <c r="AI10">
+        <v>-7.37416259470529E-2</v>
+      </c>
+      <c r="AJ10">
+        <v>-0.45752182049083201</v>
       </c>
       <c r="AK10">
-        <v>-0.70128518425964304</v>
+        <v>-0.86119702202036796</v>
       </c>
       <c r="AL10">
-        <v>1.3753239661330099</v>
+        <v>1.1024401945026301</v>
       </c>
       <c r="AM10">
-        <v>1.09717397864432</v>
-      </c>
-      <c r="AN10" s="1">
-        <v>3.0214080197765699E-6</v>
-      </c>
-      <c r="AO10" s="1">
-        <v>-5.9254279918263802E-6</v>
-      </c>
-      <c r="AP10" s="1">
-        <v>-4.7270501823959404E-6</v>
-      </c>
-      <c r="AQ10" s="1">
-        <v>4.3083870693294498E-6</v>
-      </c>
-      <c r="AR10" s="1">
-        <v>-6.1103817250440699E-7</v>
+        <v>1.68308375442707</v>
+      </c>
+      <c r="AN10">
+        <v>-0.46526629166713401</v>
+      </c>
+      <c r="AO10">
+        <v>0.59559920432342695</v>
+      </c>
+      <c r="AP10">
+        <v>0.90929498937464004</v>
+      </c>
+      <c r="AQ10">
+        <v>-0.54025534200712799</v>
+      </c>
+      <c r="AR10">
+        <v>-0.93768715052587903</v>
       </c>
       <c r="AS10">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="1">
-        <v>-3.0619896362334298E-5</v>
-      </c>
-      <c r="AU10" s="1">
-        <v>-3.0619896362334298E-5</v>
+        <v>5.3846839205937601E-2</v>
+      </c>
+      <c r="AT10">
+        <v>0.76971158768196302</v>
+      </c>
+      <c r="AU10">
+        <v>-0.62882339724816605</v>
       </c>
       <c r="AV10">
         <v>1</v>
@@ -1429,7 +1730,7 @@
         <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1438,76 +1739,76 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1.01779729316456</v>
+        <v>1.00743652030105</v>
       </c>
       <c r="F12">
-        <v>0.27341189029341401</v>
+        <v>0.34669713770872701</v>
       </c>
       <c r="G12">
-        <v>0.93711098245678404</v>
+        <v>3.9628718104648797E-2</v>
       </c>
       <c r="H12">
-        <v>0.93711098245678404</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>1.38318143328473E-2</v>
+        <v>1.5920602214279201E-2</v>
       </c>
       <c r="J12">
-        <v>0.76921262517232503</v>
+        <v>0.79357871945774905</v>
       </c>
       <c r="K12">
-        <v>1.38318143328473E-2</v>
+        <v>1.33665358108239E-2</v>
       </c>
       <c r="L12">
-        <v>2.66590222475162</v>
+        <v>2.6660361125795</v>
       </c>
       <c r="M12">
-        <v>28.0422014617989</v>
+        <v>27.899107123653199</v>
       </c>
       <c r="N12">
-        <v>30.708103686550501</v>
+        <v>30.5651432362327</v>
       </c>
       <c r="O12">
-        <v>3.4519684204854899</v>
+        <v>3.3958262504747001</v>
       </c>
       <c r="P12">
-        <v>0.2836773859476</v>
+        <v>0.41848892858679598</v>
       </c>
       <c r="Q12">
-        <v>1.3139165170151299</v>
+        <v>0.88330342779472604</v>
       </c>
       <c r="R12">
-        <v>25.6585357020621</v>
+        <v>25.867509738690401</v>
       </c>
       <c r="S12">
-        <v>3.73564580643309</v>
+        <v>3.8143151790615</v>
       </c>
       <c r="T12">
-        <v>4.76588493750062</v>
+        <v>4.2791296782694301</v>
       </c>
       <c r="U12">
-        <v>26.972452219077301</v>
+        <v>26.750813166485099</v>
       </c>
       <c r="V12">
-        <v>25.942213088009701</v>
+        <v>26.285998667277202</v>
       </c>
       <c r="W12">
-        <v>2.44191230583262</v>
+        <v>2.8106735333333299</v>
       </c>
       <c r="X12">
-        <v>8.9153378297480508</v>
+        <v>7.6678344650008396</v>
       </c>
       <c r="Y12">
-        <v>2.44191230583262</v>
+        <v>2.3597705620795701</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>0.450902971253764</v>
       </c>
       <c r="AA12">
-        <v>0.2836773859476</v>
+        <v>0.26139632019444298</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>5.1104373873961502E-2</v>
       </c>
       <c r="AC12">
         <v>38.630093333333299</v>
@@ -1516,55 +1817,55 @@
         <v>176.54316686666601</v>
       </c>
       <c r="AE12">
-        <v>27.3331676380052</v>
+        <v>28.4466895033333</v>
       </c>
       <c r="AF12">
-        <v>155.56410353199399</v>
+        <v>154.45058166666601</v>
       </c>
       <c r="AG12">
-        <v>5.7945139999999897</v>
+        <v>5.7945140000000004</v>
       </c>
       <c r="AH12">
         <v>26.481475029999999</v>
       </c>
       <c r="AI12">
-        <v>-1.17868453939012</v>
+        <v>-1.17863712757008</v>
       </c>
       <c r="AJ12">
-        <v>0.24844358073140899</v>
+        <v>0.1035444667199</v>
       </c>
       <c r="AK12">
-        <v>0.15706206482354301</v>
+        <v>6.0298283772716003E-2</v>
       </c>
       <c r="AL12">
-        <v>-0.18083758910995201</v>
+        <v>-0.29527590910741902</v>
       </c>
       <c r="AM12">
-        <v>-0.34394133513661101</v>
+        <v>-0.11425648214826201</v>
       </c>
       <c r="AN12">
-        <v>0.24625546179894101</v>
+        <v>0.103161123653269</v>
       </c>
       <c r="AO12">
-        <v>-0.28353278092268702</v>
+        <v>-0.50517183351485395</v>
       </c>
       <c r="AP12">
-        <v>-0.53926091199021897</v>
+        <v>-0.195475332722782</v>
       </c>
       <c r="AQ12">
-        <v>-1.5678863134494301</v>
+        <v>-1.71084676376722</v>
       </c>
       <c r="AR12">
-        <v>-0.81849394460894098</v>
+        <v>-0.99535441226425103</v>
       </c>
       <c r="AS12">
-        <v>3.87338798336542E-2</v>
+        <v>4.90868128069291E-2</v>
       </c>
       <c r="AT12">
-        <v>1.9611805497435399</v>
+        <v>2.1565068579520701</v>
       </c>
       <c r="AU12">
-        <v>-2.0975370440627299</v>
+        <v>-2.27228609778955</v>
       </c>
       <c r="AV12">
         <v>1</v>
@@ -1575,7 +1876,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1584,76 +1885,76 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0.96528992239972999</v>
+        <v>1.01779729316456</v>
       </c>
       <c r="F13">
-        <v>0.368354550997812</v>
+        <v>0.27341189029341401</v>
       </c>
       <c r="G13">
-        <v>0.449691507619493</v>
+        <v>0.93711098245678404</v>
       </c>
       <c r="H13">
-        <v>0.368354550997812</v>
+        <v>0.93711098245678404</v>
       </c>
       <c r="I13">
-        <v>1.42244864412924E-2</v>
+        <v>1.38318143328473E-2</v>
       </c>
       <c r="J13">
-        <v>0.79357871945774905</v>
+        <v>0.76921262517232503</v>
       </c>
       <c r="K13">
-        <v>1.31507565623004E-2</v>
+        <v>1.38318143328473E-2</v>
       </c>
       <c r="L13">
-        <v>4.4016067902035596</v>
+        <v>2.66590222475162</v>
       </c>
       <c r="M13">
-        <v>27.309285981633799</v>
+        <v>28.0422014617989</v>
       </c>
       <c r="N13">
-        <v>31.710892771837301</v>
+        <v>30.708103686550501</v>
       </c>
       <c r="O13">
-        <v>3.4479970173011201</v>
+        <v>3.4519684204854899</v>
       </c>
       <c r="P13">
-        <v>0.32250493030917898</v>
+        <v>0.2836773859476</v>
       </c>
       <c r="Q13">
-        <v>0.896873797351182</v>
+        <v>1.3139165170151299</v>
       </c>
       <c r="R13">
-        <v>27.043470610978002</v>
+        <v>25.6585357020621</v>
       </c>
       <c r="S13">
-        <v>3.7705019476102999</v>
+        <v>3.73564580643309</v>
       </c>
       <c r="T13">
-        <v>4.3448708146523103</v>
+        <v>4.76588493750062</v>
       </c>
       <c r="U13">
-        <v>27.9403444083291</v>
+        <v>26.972452219077301</v>
       </c>
       <c r="V13">
-        <v>27.365975541287099</v>
+        <v>25.942213088009701</v>
       </c>
       <c r="W13">
-        <v>2.5112358833977302</v>
+        <v>2.44191230583262</v>
       </c>
       <c r="X13">
-        <v>7.6437055715808002</v>
+        <v>8.9153378297480508</v>
       </c>
       <c r="Y13">
-        <v>2.3216762102011201</v>
+        <v>2.44191230583262</v>
       </c>
       <c r="Z13">
-        <v>0.18955967319661199</v>
+        <v>0</v>
       </c>
       <c r="AA13">
-        <v>0.26112759085858001</v>
+        <v>0.2836773859476</v>
       </c>
       <c r="AB13">
-        <v>2.1536730284274198E-2</v>
+        <v>0</v>
       </c>
       <c r="AC13">
         <v>38.630093333333299</v>
@@ -1662,57 +1963,203 @@
         <v>176.54316686666601</v>
       </c>
       <c r="AE13">
-        <v>28.192167500888001</v>
+        <v>27.3331676380052</v>
       </c>
       <c r="AF13">
-        <v>154.705103669111</v>
+        <v>155.56410353199399</v>
       </c>
       <c r="AG13">
-        <v>5.7945140000000004</v>
+        <v>5.7945139999999897</v>
       </c>
       <c r="AH13">
         <v>26.481475029999999</v>
       </c>
       <c r="AI13">
+        <v>-1.17868453939012</v>
+      </c>
+      <c r="AJ13">
+        <v>0.24844358073140899</v>
+      </c>
+      <c r="AK13">
+        <v>0.15706206482354301</v>
+      </c>
+      <c r="AL13">
+        <v>-0.18083758910995201</v>
+      </c>
+      <c r="AM13">
+        <v>-0.34394133513661101</v>
+      </c>
+      <c r="AN13">
+        <v>0.24625546179894101</v>
+      </c>
+      <c r="AO13">
+        <v>-0.28353278092268702</v>
+      </c>
+      <c r="AP13">
+        <v>-0.53926091199021897</v>
+      </c>
+      <c r="AQ13">
+        <v>-1.5678863134494301</v>
+      </c>
+      <c r="AR13">
+        <v>-0.81849394460894098</v>
+      </c>
+      <c r="AS13">
+        <v>3.87338798336542E-2</v>
+      </c>
+      <c r="AT13">
+        <v>1.9611805497435399</v>
+      </c>
+      <c r="AU13">
+        <v>-2.0975370440627299</v>
+      </c>
+      <c r="AV13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.96528992239972999</v>
+      </c>
+      <c r="F14">
+        <v>0.368354550997812</v>
+      </c>
+      <c r="G14">
+        <v>0.449691507619493</v>
+      </c>
+      <c r="H14">
+        <v>0.368354550997812</v>
+      </c>
+      <c r="I14">
+        <v>1.42244864412924E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K14">
+        <v>1.31507565623004E-2</v>
+      </c>
+      <c r="L14">
+        <v>4.4016067902035596</v>
+      </c>
+      <c r="M14">
+        <v>27.309285981633799</v>
+      </c>
+      <c r="N14">
+        <v>31.710892771837301</v>
+      </c>
+      <c r="O14">
+        <v>3.4479970173011201</v>
+      </c>
+      <c r="P14">
+        <v>0.32250493030917898</v>
+      </c>
+      <c r="Q14">
+        <v>0.896873797351182</v>
+      </c>
+      <c r="R14">
+        <v>27.043470610978002</v>
+      </c>
+      <c r="S14">
+        <v>3.7705019476102999</v>
+      </c>
+      <c r="T14">
+        <v>4.3448708146523103</v>
+      </c>
+      <c r="U14">
+        <v>27.9403444083291</v>
+      </c>
+      <c r="V14">
+        <v>27.365975541287099</v>
+      </c>
+      <c r="W14">
+        <v>2.5112358833977302</v>
+      </c>
+      <c r="X14">
+        <v>7.6437055715808002</v>
+      </c>
+      <c r="Y14">
+        <v>2.3216762102011201</v>
+      </c>
+      <c r="Z14">
+        <v>0.18955967319661199</v>
+      </c>
+      <c r="AA14">
+        <v>0.26112759085858001</v>
+      </c>
+      <c r="AB14">
+        <v>2.1536730284274198E-2</v>
+      </c>
+      <c r="AC14">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD14">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE14">
+        <v>28.192167500888001</v>
+      </c>
+      <c r="AF14">
+        <v>154.705103669111</v>
+      </c>
+      <c r="AG14">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH14">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI14">
         <v>-7.7072707683426403E-2</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ14">
         <v>-0.47818915133221501</v>
       </c>
-      <c r="AK13">
+      <c r="AK14">
         <v>-0.86119696596022099</v>
       </c>
-      <c r="AL13">
+      <c r="AL14">
         <v>1.2110471866130601</v>
       </c>
-      <c r="AM13">
+      <c r="AM14">
         <v>1.5652201023230701</v>
       </c>
-      <c r="AN13">
+      <c r="AN14">
         <v>-0.48666001836618</v>
       </c>
-      <c r="AO13">
+      <c r="AO14">
         <v>0.68435940832918596</v>
       </c>
-      <c r="AP13">
+      <c r="AP14">
         <v>0.88450154128718195</v>
       </c>
-      <c r="AQ13">
+      <c r="AQ14">
         <v>-0.56509722816262098</v>
       </c>
-      <c r="AR13">
+      <c r="AR14">
         <v>-0.93776637042770805</v>
       </c>
-      <c r="AS13">
+      <c r="AS14">
         <v>5.4140992846667103E-2</v>
       </c>
-      <c r="AT13">
+      <c r="AT14">
         <v>0.80643693546159301</v>
       </c>
-      <c r="AU13">
+      <c r="AU14">
         <v>-0.65640513572710901</v>
       </c>
-      <c r="AV13">
+      <c r="AV14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add analytical forms for production tax
</commit_message>
<xml_diff>
--- a/Data/output/temp.xlsx
+++ b/Data/output/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Tobin\sam\Optimal-Unilateral-Carbon-Policy\Data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3986DBD3-7E6D-477D-B476-91ED94B0E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6455A23D-4C5C-4E44-A761-8E5D1B395A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14424" yWindow="2760" windowWidth="15384" windowHeight="11088" xr2:uid="{36D558F1-4F96-478A-B61D-823EAD2C98E9}"/>
+    <workbookView xWindow="11232" yWindow="2784" windowWidth="15384" windowHeight="11088" xr2:uid="{36D558F1-4F96-478A-B61D-823EAD2C98E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>PC_hybrid</t>
   </si>
@@ -552,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3496870A-4D61-430B-B032-0A96A329A70C}">
-  <dimension ref="A1:AV18"/>
+  <dimension ref="A1:AV23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2309,30 +2309,176 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1.10475352601461</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1.10475352601461</v>
+      </c>
+      <c r="I17">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="J17">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K17">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>29.2155561149448</v>
+      </c>
+      <c r="N17">
+        <v>29.2155561149448</v>
+      </c>
+      <c r="O17">
+        <v>4.1623791114645199</v>
+      </c>
+      <c r="P17">
+        <v>0.38162451630357902</v>
+      </c>
+      <c r="Q17">
+        <v>1.0826948924208899</v>
+      </c>
+      <c r="R17">
+        <v>23.588857954598001</v>
+      </c>
+      <c r="S17">
+        <v>4.5440036277680997</v>
+      </c>
+      <c r="T17">
+        <v>5.2450740038854198</v>
+      </c>
+      <c r="U17">
+        <v>24.671552847018901</v>
+      </c>
+      <c r="V17">
+        <v>23.970482470901601</v>
+      </c>
+      <c r="W17">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="X17">
+        <v>7.9740733333333296</v>
+      </c>
+      <c r="Y17">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0.38162451630357902</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD17">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE17">
+        <v>28.4466895033333</v>
+      </c>
+      <c r="AF17">
+        <v>154.45058166666601</v>
+      </c>
+      <c r="AG17">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH17">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI17">
+        <v>-1.49334826666666</v>
+      </c>
+      <c r="AJ17">
+        <v>1.49334754415436</v>
+      </c>
+      <c r="AK17">
+        <v>0.46385910242242701</v>
+      </c>
+      <c r="AL17">
+        <v>-0.844465931971768</v>
+      </c>
+      <c r="AM17">
+        <v>-0.82046913065503102</v>
+      </c>
+      <c r="AN17">
+        <v>1.4196101149448499</v>
+      </c>
+      <c r="AO17">
+        <v>-2.5844321529810599</v>
+      </c>
+      <c r="AP17">
+        <v>-2.5109915290983902</v>
+      </c>
+      <c r="AQ17">
+        <v>-3.06043388505514</v>
+      </c>
+      <c r="AR17">
+        <v>-0.29442796309261399</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>7.5212363129743496</v>
+      </c>
+      <c r="AU17">
+        <v>-8.32358195911881</v>
+      </c>
+      <c r="AV17">
+        <v>1</v>
+      </c>
+    </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>0.99999966741491597</v>
+        <v>0.94764505379350505</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.71973824850731705</v>
       </c>
       <c r="G18">
-        <v>0.77078593725241795</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>0.71973824850731705</v>
       </c>
       <c r="I18">
         <v>1.5920602214279201E-2</v>
@@ -2341,58 +2487,58 @@
         <v>0.79357871945774905</v>
       </c>
       <c r="K18">
-        <v>1.5920602214279201E-2</v>
+        <v>1.13951031352846E-2</v>
       </c>
       <c r="L18">
-        <v>4.4800440550019003</v>
+        <v>4.3611920024076998</v>
       </c>
       <c r="M18">
-        <v>27.795941377740998</v>
+        <v>27.058536868773299</v>
       </c>
       <c r="N18">
-        <v>32.275985432742999</v>
+        <v>31.419728871181</v>
       </c>
       <c r="O18">
-        <v>4.5984045293607503</v>
+        <v>2.7578559732814001</v>
       </c>
       <c r="P18">
-        <v>0.42160117021825999</v>
+        <v>0.44489340002598399</v>
       </c>
       <c r="Q18">
-        <v>1.1961113978088</v>
+        <v>0.71735814935263198</v>
       </c>
       <c r="R18">
-        <v>26.0598826671282</v>
+        <v>27.499614856512</v>
       </c>
       <c r="S18">
-        <v>5.0200056995790101</v>
+        <v>3.20274937330738</v>
       </c>
       <c r="T18">
-        <v>5.7945159271695603</v>
+        <v>3.4752141226340298</v>
       </c>
       <c r="U18">
-        <v>27.255994064936999</v>
+        <v>28.216973005864599</v>
       </c>
       <c r="V18">
-        <v>26.481483837346499</v>
+        <v>27.944508256537901</v>
       </c>
       <c r="W18">
         <v>2.8106735333333299</v>
       </c>
       <c r="X18">
-        <v>7.9740733333333296</v>
+        <v>7.4577632353658103</v>
       </c>
       <c r="Y18">
-        <v>2.8106735333333299</v>
+        <v>2.01172759427542</v>
       </c>
       <c r="Z18">
-        <v>0</v>
+        <v>0.79894593905790501</v>
       </c>
       <c r="AA18">
-        <v>0.42160117021825999</v>
+        <v>0.18097766645792601</v>
       </c>
       <c r="AB18">
-        <v>0</v>
+        <v>7.51824449577949E-2</v>
       </c>
       <c r="AC18">
         <v>38.630093333333299</v>
@@ -2407,51 +2553,781 @@
         <v>154.45058166666601</v>
       </c>
       <c r="AG18">
-        <v>5.7945140000000004</v>
+        <v>5.7945139999999897</v>
       </c>
       <c r="AH18">
         <v>26.481475029999999</v>
       </c>
-      <c r="AI18" s="1">
-        <v>-7.44997975873844E-7</v>
-      </c>
-      <c r="AJ18" s="1">
-        <v>-4.6222581317710596E-6</v>
+      <c r="AI18">
+        <v>-0.11572759009151599</v>
+      </c>
+      <c r="AJ18">
+        <v>-0.71801912447257599</v>
       </c>
       <c r="AK18">
-        <v>-1.0120426552933699</v>
+        <v>-0.86119655138820606</v>
       </c>
       <c r="AL18">
-        <v>1.98476614578185</v>
+        <v>1.12230717186722</v>
       </c>
       <c r="AM18">
-        <v>2.15388503924502</v>
-      </c>
-      <c r="AN18" s="1">
-        <v>-4.62225890274226E-6</v>
-      </c>
-      <c r="AO18" s="1">
-        <v>9.0649370747541895E-6</v>
-      </c>
-      <c r="AP18" s="1">
-        <v>9.8373465249323999E-6</v>
-      </c>
-      <c r="AQ18" s="1">
-        <v>-4.5672570010424301E-6</v>
-      </c>
-      <c r="AR18" s="1">
-        <v>9.3478809315428095E-7</v>
+        <v>1.70863093897064</v>
+      </c>
+      <c r="AN18">
+        <v>-0.73740913122665497</v>
+      </c>
+      <c r="AO18">
+        <v>0.96098800586463895</v>
+      </c>
+      <c r="AP18">
+        <v>1.4630342565379899</v>
+      </c>
+      <c r="AQ18">
+        <v>-0.856261128818953</v>
+      </c>
+      <c r="AR18">
+        <v>-1.87579658436552</v>
       </c>
       <c r="AS18">
-        <v>0</v>
-      </c>
-      <c r="AT18" s="1">
-        <v>3.8308054920663503E-5</v>
-      </c>
-      <c r="AU18" s="1">
-        <v>3.8308054920663503E-5</v>
+        <v>0.102273725844858</v>
+      </c>
+      <c r="AT18">
+        <v>2.6089475368670998</v>
+      </c>
+      <c r="AU18">
+        <v>-1.8241826953676701</v>
       </c>
       <c r="AV18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>120</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0.96549694971196298</v>
+      </c>
+      <c r="F19">
+        <v>0.53334917081631705</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1.3796019032117001E-8</v>
+      </c>
+      <c r="H19">
+        <v>0.53334917081631705</v>
+      </c>
+      <c r="I19">
+        <v>1.22733309874713E-2</v>
+      </c>
+      <c r="J19">
+        <v>0.74701382916840098</v>
+      </c>
+      <c r="K19">
+        <v>1.22733309874713E-2</v>
+      </c>
+      <c r="L19">
+        <v>4.40207877481041</v>
+      </c>
+      <c r="M19">
+        <v>27.312214358297499</v>
+      </c>
+      <c r="N19">
+        <v>31.714293133108001</v>
+      </c>
+      <c r="O19">
+        <v>2.88794295293253</v>
+      </c>
+      <c r="P19">
+        <v>0.216844080008088</v>
+      </c>
+      <c r="Q19">
+        <v>1.5183185292583401</v>
+      </c>
+      <c r="R19">
+        <v>27.091187734693101</v>
+      </c>
+      <c r="S19">
+        <v>3.1047870329406102</v>
+      </c>
+      <c r="T19">
+        <v>4.4062614821908701</v>
+      </c>
+      <c r="U19">
+        <v>28.609506263951399</v>
+      </c>
+      <c r="V19">
+        <v>27.308031814701199</v>
+      </c>
+      <c r="W19">
+        <v>2.1667727205309801</v>
+      </c>
+      <c r="X19">
+        <v>9.77287939126726</v>
+      </c>
+      <c r="Y19">
+        <v>2.1667727205309801</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0.216844080008088</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD19">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE19">
+        <v>26.3703886632075</v>
+      </c>
+      <c r="AF19">
+        <v>156.52688250679199</v>
+      </c>
+      <c r="AG19">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH19">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI19">
+        <v>-7.6617056842922596E-2</v>
+      </c>
+      <c r="AJ19">
+        <v>-0.47536211572812997</v>
+      </c>
+      <c r="AK19">
+        <v>-0.86119697334082501</v>
+      </c>
+      <c r="AL19">
+        <v>2.40970057647078</v>
+      </c>
+      <c r="AM19">
+        <v>1.4715371642977999</v>
+      </c>
+      <c r="AN19">
+        <v>-0.48373164170240501</v>
+      </c>
+      <c r="AO19">
+        <v>1.35352126395146</v>
+      </c>
+      <c r="AP19">
+        <v>0.82655781470120004</v>
+      </c>
+      <c r="AQ19">
+        <v>-0.56169686689198794</v>
+      </c>
+      <c r="AR19">
+        <v>-1.40209358817484</v>
+      </c>
+      <c r="AS19">
+        <v>7.6520733857822695E-2</v>
+      </c>
+      <c r="AT19">
+        <v>1.76258483469937</v>
+      </c>
+      <c r="AU19">
+        <v>-1.1454945795851501</v>
+      </c>
+      <c r="AV19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>120</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>1.05020999806624</v>
+      </c>
+      <c r="F20">
+        <v>0.72191181624733303</v>
+      </c>
+      <c r="G20">
+        <v>2.6005530520067599E-2</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>1.5920602214279201E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K20">
+        <v>1.1681425813631E-2</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>28.485217083806099</v>
+      </c>
+      <c r="N20">
+        <v>28.485217083806099</v>
+      </c>
+      <c r="O20">
+        <v>2.5948571722656402</v>
+      </c>
+      <c r="P20">
+        <v>0.40144450231505502</v>
+      </c>
+      <c r="Q20">
+        <v>0.67495980825861202</v>
+      </c>
+      <c r="R20">
+        <v>24.813964871772299</v>
+      </c>
+      <c r="S20">
+        <v>2.9963016745806899</v>
+      </c>
+      <c r="T20">
+        <v>3.2698169805242498</v>
+      </c>
+      <c r="U20">
+        <v>25.488924680030902</v>
+      </c>
+      <c r="V20">
+        <v>25.2154093740874</v>
+      </c>
+      <c r="W20">
+        <v>2.8106735333333299</v>
+      </c>
+      <c r="X20">
+        <v>7.4868118722594001</v>
+      </c>
+      <c r="Y20">
+        <v>2.0622759066564398</v>
+      </c>
+      <c r="Z20">
+        <v>0.74839762667686904</v>
+      </c>
+      <c r="AA20">
+        <v>0.174559888321384</v>
+      </c>
+      <c r="AB20">
+        <v>6.6031019361389998E-2</v>
+      </c>
+      <c r="AC20">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD20">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE20">
+        <v>28.4466895033333</v>
+      </c>
+      <c r="AF20">
+        <v>154.45058166666601</v>
+      </c>
+      <c r="AG20">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH20">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI20">
+        <v>-1.49334826666666</v>
+      </c>
+      <c r="AJ20">
+        <v>0.70650459283358502</v>
+      </c>
+      <c r="AK20">
+        <v>0.181828639975159</v>
+      </c>
+      <c r="AL20">
+        <v>-0.46614776433067601</v>
+      </c>
+      <c r="AM20">
+        <v>-0.33398587937148</v>
+      </c>
+      <c r="AN20">
+        <v>0.68927108380618995</v>
+      </c>
+      <c r="AO20">
+        <v>-1.76706031996902</v>
+      </c>
+      <c r="AP20">
+        <v>-1.2660646259125801</v>
+      </c>
+      <c r="AQ20">
+        <v>-3.7907729161938</v>
+      </c>
+      <c r="AR20">
+        <v>-2.1701823480004898</v>
+      </c>
+      <c r="AS20">
+        <v>9.3471794824297294E-2</v>
+      </c>
+      <c r="AT20">
+        <v>9.7218670389514408</v>
+      </c>
+      <c r="AU20">
+        <v>-9.9041435934531794</v>
+      </c>
+      <c r="AV20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>1.06857546542679</v>
+      </c>
+      <c r="F21">
+        <v>0.54080646625754403</v>
+      </c>
+      <c r="G21">
+        <v>1.83765666997987</v>
+      </c>
+      <c r="H21">
+        <v>1.6093819316843401</v>
+      </c>
+      <c r="I21">
+        <v>1.24955707128776E-2</v>
+      </c>
+      <c r="J21">
+        <v>0.75043234141008797</v>
+      </c>
+      <c r="K21">
+        <v>1.24955707128776E-2</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>28.7332041510846</v>
+      </c>
+      <c r="N21">
+        <v>28.7332041510846</v>
+      </c>
+      <c r="O21">
+        <v>2.70190151554455</v>
+      </c>
+      <c r="P21">
+        <v>0.20560762864789001</v>
+      </c>
+      <c r="Q21">
+        <v>1.3533188234570399</v>
+      </c>
+      <c r="R21">
+        <v>24.472369741089299</v>
+      </c>
+      <c r="S21">
+        <v>2.9075091441924399</v>
+      </c>
+      <c r="T21">
+        <v>4.0552203390016004</v>
+      </c>
+      <c r="U21">
+        <v>25.8256885645464</v>
+      </c>
+      <c r="V21">
+        <v>24.677977369737199</v>
+      </c>
+      <c r="W21">
+        <v>2.2060076254577901</v>
+      </c>
+      <c r="X21">
+        <v>9.6408219443097494</v>
+      </c>
+      <c r="Y21">
+        <v>2.2060076254577901</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0.20560762864789001</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD21">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE21">
+        <v>26.515987162309099</v>
+      </c>
+      <c r="AF21">
+        <v>156.38128400769</v>
+      </c>
+      <c r="AG21">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH21">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI21">
+        <v>-1.49334826666666</v>
+      </c>
+      <c r="AJ21">
+        <v>0.96921699964950903</v>
+      </c>
+      <c r="AK21">
+        <v>0.26455399537389102</v>
+      </c>
+      <c r="AL21">
+        <v>-0.403720827746744</v>
+      </c>
+      <c r="AM21">
+        <v>-0.509061712215788</v>
+      </c>
+      <c r="AN21">
+        <v>0.93725815108464094</v>
+      </c>
+      <c r="AO21">
+        <v>-1.4302964354535499</v>
+      </c>
+      <c r="AP21">
+        <v>-1.80349663026271</v>
+      </c>
+      <c r="AQ21">
+        <v>-3.5427858489153499</v>
+      </c>
+      <c r="AR21">
+        <v>-1.7127728640452899</v>
+      </c>
+      <c r="AS21">
+        <v>7.0558564514069499E-2</v>
+      </c>
+      <c r="AT21">
+        <v>9.0149986889675393</v>
+      </c>
+      <c r="AU21">
+        <v>-9.3271057515588005</v>
+      </c>
+      <c r="AV21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>0.94546350130836998</v>
+      </c>
+      <c r="F22">
+        <v>0.72198195570280799</v>
+      </c>
+      <c r="G22">
+        <v>0.51081433172528101</v>
+      </c>
+      <c r="H22">
+        <v>0.72198195570280799</v>
+      </c>
+      <c r="I22">
+        <v>1.3196304514679799E-2</v>
+      </c>
+      <c r="J22">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K22">
+        <v>1.1379284494828199E-2</v>
+      </c>
+      <c r="L22">
+        <v>4.3561692087395096</v>
+      </c>
+      <c r="M22">
+        <v>27.0273734970208</v>
+      </c>
+      <c r="N22">
+        <v>31.383542705760298</v>
+      </c>
+      <c r="O22">
+        <v>2.7577533704120598</v>
+      </c>
+      <c r="P22">
+        <v>0.26909362891803001</v>
+      </c>
+      <c r="Q22">
+        <v>0.71733146086520605</v>
+      </c>
+      <c r="R22">
+        <v>27.6393719962152</v>
+      </c>
+      <c r="S22">
+        <v>3.0268469993300902</v>
+      </c>
+      <c r="T22">
+        <v>3.47508483127727</v>
+      </c>
+      <c r="U22">
+        <v>28.3567034570804</v>
+      </c>
+      <c r="V22">
+        <v>27.908465625133299</v>
+      </c>
+      <c r="W22">
+        <v>2.3297173899584598</v>
+      </c>
+      <c r="X22">
+        <v>7.45617304792159</v>
+      </c>
+      <c r="Y22">
+        <v>2.0089349213937302</v>
+      </c>
+      <c r="Z22">
+        <v>0.32078246856471898</v>
+      </c>
+      <c r="AA22">
+        <v>0.18071971020413199</v>
+      </c>
+      <c r="AB22">
+        <v>2.9418206135427099E-2</v>
+      </c>
+      <c r="AC22">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD22">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE22">
+        <v>28.0378767814646</v>
+      </c>
+      <c r="AF22">
+        <v>154.85939438853501</v>
+      </c>
+      <c r="AG22">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH22">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI22">
+        <v>-0.120481935871141</v>
+      </c>
+      <c r="AJ22">
+        <v>-0.74751694077919095</v>
+      </c>
+      <c r="AK22">
+        <v>-0.86119651876357195</v>
+      </c>
+      <c r="AL22">
+        <v>1.2333708266977801</v>
+      </c>
+      <c r="AM22">
+        <v>1.5989645935888801</v>
+      </c>
+      <c r="AN22">
+        <v>-0.76857250297911495</v>
+      </c>
+      <c r="AO22">
+        <v>1.10071845708049</v>
+      </c>
+      <c r="AP22">
+        <v>1.4269916251333199</v>
+      </c>
+      <c r="AQ22">
+        <v>-0.89244729423960201</v>
+      </c>
+      <c r="AR22">
+        <v>-1.87597094559966</v>
+      </c>
+      <c r="AS22">
+        <v>0.10277216408643999</v>
+      </c>
+      <c r="AT22">
+        <v>2.7265401491498702</v>
+      </c>
+      <c r="AU22">
+        <v>-1.8939371183709599</v>
+      </c>
+      <c r="AV22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>120</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>1.0479041150056301</v>
+      </c>
+      <c r="F23">
+        <v>0.72428040832501495</v>
+      </c>
+      <c r="G23">
+        <v>0.50028625973930496</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>1.33591888964994E-2</v>
+      </c>
+      <c r="J23">
+        <v>0.79357871945774905</v>
+      </c>
+      <c r="K23">
+        <v>1.1665966775076199E-2</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>28.453928258865702</v>
+      </c>
+      <c r="N23">
+        <v>28.453928258865702</v>
+      </c>
+      <c r="O23">
+        <v>2.59476604250343</v>
+      </c>
+      <c r="P23">
+        <v>0.25093052162003399</v>
+      </c>
+      <c r="Q23">
+        <v>0.67493610409196902</v>
+      </c>
+      <c r="R23">
+        <v>24.933296499819399</v>
+      </c>
+      <c r="S23">
+        <v>2.8456965641234602</v>
+      </c>
+      <c r="T23">
+        <v>3.2697021465953999</v>
+      </c>
+      <c r="U23">
+        <v>25.608232603911301</v>
+      </c>
+      <c r="V23">
+        <v>25.184227021439401</v>
+      </c>
+      <c r="W23">
+        <v>2.35847351455801</v>
+      </c>
+      <c r="X23">
+        <v>7.4852306541771698</v>
+      </c>
+      <c r="Y23">
+        <v>2.0595467190332801</v>
+      </c>
+      <c r="Z23">
+        <v>0.29892679552474699</v>
+      </c>
+      <c r="AA23">
+        <v>0.17432275584035101</v>
+      </c>
+      <c r="AB23">
+        <v>2.57504710539691E-2</v>
+      </c>
+      <c r="AC23">
+        <v>38.630093333333299</v>
+      </c>
+      <c r="AD23">
+        <v>176.54316686666601</v>
+      </c>
+      <c r="AE23">
+        <v>28.0623194873743</v>
+      </c>
+      <c r="AF23">
+        <v>154.83495168262499</v>
+      </c>
+      <c r="AG23">
+        <v>5.7945140000000004</v>
+      </c>
+      <c r="AH23">
+        <v>26.481475029999999</v>
+      </c>
+      <c r="AI23">
+        <v>-1.49334826666666</v>
+      </c>
+      <c r="AJ23">
+        <v>0.67368083684680602</v>
+      </c>
+      <c r="AK23">
+        <v>0.172153749319193</v>
+      </c>
+      <c r="AL23">
+        <v>-0.43111611158840002</v>
+      </c>
+      <c r="AM23">
+        <v>-0.339410262424371</v>
+      </c>
+      <c r="AN23">
+        <v>0.65798225886571104</v>
+      </c>
+      <c r="AO23">
+        <v>-1.6477523960886</v>
+      </c>
+      <c r="AP23">
+        <v>-1.2972469785605401</v>
+      </c>
+      <c r="AQ23">
+        <v>-3.8220617411342799</v>
+      </c>
+      <c r="AR23">
+        <v>-2.1703572786896701</v>
+      </c>
+      <c r="AS23">
+        <v>9.3936584170300999E-2</v>
+      </c>
+      <c r="AT23">
+        <v>9.8219856631442504</v>
+      </c>
+      <c r="AU23">
+        <v>-9.9660169494008901</v>
+      </c>
+      <c r="AV23">
         <v>1</v>
       </c>
     </row>

</xml_diff>